<commit_message>
a lot of figures
</commit_message>
<xml_diff>
--- a/script/new_offloading.xlsx
+++ b/script/new_offloading.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20359"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\BandwidthUNcertinity\script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE098E41-FB0D-4154-9730-860D4F9C4547}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8ED58C-5C03-4747-8613-8935FF325BA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{60046224-DB48-4D55-9DB3-CD82E3B77A28}"/>
   </bookViews>
@@ -388,8 +388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED42AF60-AB6E-40CA-87F9-E205799F0A91}">
   <dimension ref="A1:O62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,13 +405,13 @@
         <v>100000</v>
       </c>
       <c r="C1">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D1">
         <v>30</v>
       </c>
       <c r="E1">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F1">
         <v>10</v>
@@ -420,7 +420,7 @@
         <v>24</v>
       </c>
       <c r="H1">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="I1">
         <v>1</v>
@@ -434,13 +434,13 @@
         <v>100000</v>
       </c>
       <c r="C2">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D2">
         <v>60</v>
       </c>
       <c r="E2">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F2">
         <v>10</v>
@@ -449,7 +449,7 @@
         <v>24</v>
       </c>
       <c r="H2">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -463,13 +463,13 @@
         <v>100000</v>
       </c>
       <c r="C3">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D3">
         <v>90</v>
       </c>
       <c r="E3">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F3">
         <v>10</v>
@@ -478,7 +478,7 @@
         <v>24</v>
       </c>
       <c r="H3">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -492,13 +492,13 @@
         <v>100000</v>
       </c>
       <c r="C4">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D4">
         <v>120</v>
       </c>
       <c r="E4">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F4">
         <v>10</v>
@@ -507,7 +507,7 @@
         <v>24</v>
       </c>
       <c r="H4">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -521,13 +521,13 @@
         <v>100000</v>
       </c>
       <c r="C5">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D5">
         <v>150</v>
       </c>
       <c r="E5">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F5">
         <v>10</v>
@@ -536,7 +536,7 @@
         <v>24</v>
       </c>
       <c r="H5">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -550,13 +550,13 @@
         <v>100000</v>
       </c>
       <c r="C6">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D6">
         <v>180</v>
       </c>
       <c r="E6">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F6">
         <v>10</v>
@@ -565,7 +565,7 @@
         <v>24</v>
       </c>
       <c r="H6">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -579,13 +579,13 @@
         <v>100000</v>
       </c>
       <c r="C7">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D7">
         <v>210</v>
       </c>
       <c r="E7">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F7">
         <v>10</v>
@@ -594,7 +594,7 @@
         <v>24</v>
       </c>
       <c r="H7">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -608,13 +608,13 @@
         <v>100000</v>
       </c>
       <c r="C8">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D8">
         <v>240</v>
       </c>
       <c r="E8">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F8">
         <v>10</v>
@@ -623,7 +623,7 @@
         <v>24</v>
       </c>
       <c r="H8">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -637,13 +637,13 @@
         <v>100000</v>
       </c>
       <c r="C9">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D9">
         <v>270</v>
       </c>
       <c r="E9">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F9">
         <v>10</v>
@@ -652,7 +652,7 @@
         <v>24</v>
       </c>
       <c r="H9">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -666,13 +666,13 @@
         <v>100000</v>
       </c>
       <c r="C10">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D10">
         <v>300</v>
       </c>
       <c r="E10">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F10">
         <v>10</v>
@@ -681,7 +681,7 @@
         <v>24</v>
       </c>
       <c r="H10">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -695,13 +695,13 @@
         <v>100000</v>
       </c>
       <c r="C11">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D11">
         <v>330</v>
       </c>
       <c r="E11">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F11">
         <v>10</v>
@@ -710,7 +710,7 @@
         <v>24</v>
       </c>
       <c r="H11">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -724,13 +724,13 @@
         <v>100000</v>
       </c>
       <c r="C12">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D12">
         <v>360</v>
       </c>
       <c r="E12">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F12">
         <v>10</v>
@@ -739,7 +739,7 @@
         <v>24</v>
       </c>
       <c r="H12">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -753,13 +753,13 @@
         <v>100000</v>
       </c>
       <c r="C13">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D13">
         <v>390</v>
       </c>
       <c r="E13">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F13">
         <v>10</v>
@@ -768,7 +768,7 @@
         <v>24</v>
       </c>
       <c r="H13">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -782,13 +782,13 @@
         <v>100000</v>
       </c>
       <c r="C14">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D14">
         <v>420</v>
       </c>
       <c r="E14">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F14">
         <v>10</v>
@@ -797,7 +797,7 @@
         <v>24</v>
       </c>
       <c r="H14">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="I14">
         <v>1</v>
@@ -811,13 +811,13 @@
         <v>100000</v>
       </c>
       <c r="C15">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D15">
         <v>450</v>
       </c>
       <c r="E15">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F15">
         <v>10</v>
@@ -826,7 +826,7 @@
         <v>24</v>
       </c>
       <c r="H15">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -840,13 +840,13 @@
         <v>100000</v>
       </c>
       <c r="C16">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D16">
         <v>480</v>
       </c>
       <c r="E16">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F16">
         <v>10</v>
@@ -855,7 +855,7 @@
         <v>24</v>
       </c>
       <c r="H16">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="I16">
         <v>1</v>
@@ -869,13 +869,13 @@
         <v>100000</v>
       </c>
       <c r="C17">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D17">
         <v>510</v>
       </c>
       <c r="E17">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F17">
         <v>10</v>
@@ -884,7 +884,7 @@
         <v>24</v>
       </c>
       <c r="H17">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="I17">
         <v>1</v>
@@ -898,13 +898,13 @@
         <v>100000</v>
       </c>
       <c r="C18">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D18">
         <v>540</v>
       </c>
       <c r="E18">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F18">
         <v>10</v>
@@ -913,7 +913,7 @@
         <v>24</v>
       </c>
       <c r="H18">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="I18">
         <v>1</v>
@@ -927,13 +927,13 @@
         <v>100000</v>
       </c>
       <c r="C19">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D19">
         <v>570</v>
       </c>
       <c r="E19">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F19">
         <v>10</v>
@@ -942,7 +942,7 @@
         <v>24</v>
       </c>
       <c r="H19">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="I19">
         <v>1</v>
@@ -956,13 +956,13 @@
         <v>100000</v>
       </c>
       <c r="C20">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D20">
         <v>600</v>
       </c>
       <c r="E20">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F20">
         <v>10</v>
@@ -971,7 +971,7 @@
         <v>24</v>
       </c>
       <c r="H20">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="I20">
         <v>1</v>
@@ -985,19 +985,19 @@
         <v>100000</v>
       </c>
       <c r="C22">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D22">
         <v>30</v>
       </c>
       <c r="E22">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F22">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G22">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H22">
         <v>10</v>
@@ -1006,13 +1006,13 @@
         <v>24</v>
       </c>
       <c r="J22">
-        <v>0.64</v>
+        <v>4</v>
       </c>
       <c r="K22">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="L22">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="M22">
         <v>2</v>
@@ -1026,19 +1026,19 @@
         <v>100000</v>
       </c>
       <c r="C23">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D23">
         <v>60</v>
       </c>
       <c r="E23">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F23">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G23">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H23">
         <v>10</v>
@@ -1047,13 +1047,13 @@
         <v>24</v>
       </c>
       <c r="J23">
-        <v>0.64</v>
+        <v>4</v>
       </c>
       <c r="K23">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="L23">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="M23">
         <v>2</v>
@@ -1067,19 +1067,19 @@
         <v>100000</v>
       </c>
       <c r="C24">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D24">
         <v>90</v>
       </c>
       <c r="E24">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F24">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G24">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H24">
         <v>10</v>
@@ -1088,13 +1088,13 @@
         <v>24</v>
       </c>
       <c r="J24">
-        <v>0.64</v>
+        <v>4</v>
       </c>
       <c r="K24">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="L24">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="M24">
         <v>2</v>
@@ -1108,19 +1108,19 @@
         <v>100000</v>
       </c>
       <c r="C25">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D25">
         <v>120</v>
       </c>
       <c r="E25">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F25">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G25">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H25">
         <v>10</v>
@@ -1129,13 +1129,13 @@
         <v>24</v>
       </c>
       <c r="J25">
-        <v>0.64</v>
+        <v>4</v>
       </c>
       <c r="K25">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="L25">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="M25">
         <v>2</v>
@@ -1149,19 +1149,19 @@
         <v>100000</v>
       </c>
       <c r="C26">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D26">
         <v>150</v>
       </c>
       <c r="E26">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F26">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G26">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H26">
         <v>10</v>
@@ -1170,13 +1170,13 @@
         <v>24</v>
       </c>
       <c r="J26">
-        <v>0.64</v>
+        <v>4</v>
       </c>
       <c r="K26">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="L26">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="M26">
         <v>2</v>
@@ -1190,19 +1190,19 @@
         <v>100000</v>
       </c>
       <c r="C27">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D27">
         <v>180</v>
       </c>
       <c r="E27">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F27">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G27">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H27">
         <v>10</v>
@@ -1211,13 +1211,13 @@
         <v>24</v>
       </c>
       <c r="J27">
-        <v>0.64</v>
+        <v>4</v>
       </c>
       <c r="K27">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="L27">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="M27">
         <v>2</v>
@@ -1231,19 +1231,19 @@
         <v>100000</v>
       </c>
       <c r="C28">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D28">
         <v>210</v>
       </c>
       <c r="E28">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F28">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G28">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H28">
         <v>10</v>
@@ -1252,13 +1252,13 @@
         <v>24</v>
       </c>
       <c r="J28">
-        <v>0.64</v>
+        <v>4</v>
       </c>
       <c r="K28">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="L28">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="M28">
         <v>2</v>
@@ -1272,19 +1272,19 @@
         <v>100000</v>
       </c>
       <c r="C29">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D29">
         <v>240</v>
       </c>
       <c r="E29">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F29">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G29">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H29">
         <v>10</v>
@@ -1293,13 +1293,13 @@
         <v>24</v>
       </c>
       <c r="J29">
-        <v>0.64</v>
+        <v>4</v>
       </c>
       <c r="K29">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="L29">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="M29">
         <v>2</v>
@@ -1313,19 +1313,19 @@
         <v>100000</v>
       </c>
       <c r="C30">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D30">
         <v>270</v>
       </c>
       <c r="E30">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F30">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G30">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H30">
         <v>10</v>
@@ -1334,13 +1334,13 @@
         <v>24</v>
       </c>
       <c r="J30">
-        <v>0.64</v>
+        <v>4</v>
       </c>
       <c r="K30">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="L30">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="M30">
         <v>2</v>
@@ -1354,19 +1354,19 @@
         <v>100000</v>
       </c>
       <c r="C31">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D31">
         <v>300</v>
       </c>
       <c r="E31">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F31">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G31">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H31">
         <v>10</v>
@@ -1375,13 +1375,13 @@
         <v>24</v>
       </c>
       <c r="J31">
-        <v>0.64</v>
+        <v>4</v>
       </c>
       <c r="K31">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="L31">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="M31">
         <v>2</v>
@@ -1395,19 +1395,19 @@
         <v>100000</v>
       </c>
       <c r="C32">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D32">
         <v>330</v>
       </c>
       <c r="E32">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F32">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G32">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H32">
         <v>10</v>
@@ -1416,13 +1416,13 @@
         <v>24</v>
       </c>
       <c r="J32">
-        <v>0.64</v>
+        <v>4</v>
       </c>
       <c r="K32">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="L32">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="M32">
         <v>2</v>
@@ -1436,19 +1436,19 @@
         <v>100000</v>
       </c>
       <c r="C33">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D33">
         <v>360</v>
       </c>
       <c r="E33">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F33">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G33">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H33">
         <v>10</v>
@@ -1457,13 +1457,13 @@
         <v>24</v>
       </c>
       <c r="J33">
-        <v>0.64</v>
+        <v>4</v>
       </c>
       <c r="K33">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="L33">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="M33">
         <v>2</v>
@@ -1477,19 +1477,19 @@
         <v>100000</v>
       </c>
       <c r="C34">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D34">
         <v>390</v>
       </c>
       <c r="E34">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F34">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G34">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H34">
         <v>10</v>
@@ -1498,13 +1498,13 @@
         <v>24</v>
       </c>
       <c r="J34">
-        <v>0.64</v>
+        <v>4</v>
       </c>
       <c r="K34">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="L34">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="M34">
         <v>2</v>
@@ -1518,19 +1518,19 @@
         <v>100000</v>
       </c>
       <c r="C35">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D35">
         <v>420</v>
       </c>
       <c r="E35">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F35">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G35">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H35">
         <v>10</v>
@@ -1539,13 +1539,13 @@
         <v>24</v>
       </c>
       <c r="J35">
-        <v>0.64</v>
+        <v>4</v>
       </c>
       <c r="K35">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="L35">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="M35">
         <v>2</v>
@@ -1559,19 +1559,19 @@
         <v>100000</v>
       </c>
       <c r="C36">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D36">
         <v>450</v>
       </c>
       <c r="E36">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F36">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G36">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H36">
         <v>10</v>
@@ -1580,13 +1580,13 @@
         <v>24</v>
       </c>
       <c r="J36">
-        <v>0.64</v>
+        <v>4</v>
       </c>
       <c r="K36">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="L36">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="M36">
         <v>2</v>
@@ -1600,19 +1600,19 @@
         <v>100000</v>
       </c>
       <c r="C37">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D37">
         <v>480</v>
       </c>
       <c r="E37">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F37">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G37">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H37">
         <v>10</v>
@@ -1621,13 +1621,13 @@
         <v>24</v>
       </c>
       <c r="J37">
-        <v>0.64</v>
+        <v>4</v>
       </c>
       <c r="K37">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="L37">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="M37">
         <v>2</v>
@@ -1641,19 +1641,19 @@
         <v>100000</v>
       </c>
       <c r="C38">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D38">
         <v>510</v>
       </c>
       <c r="E38">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F38">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G38">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H38">
         <v>10</v>
@@ -1662,13 +1662,13 @@
         <v>24</v>
       </c>
       <c r="J38">
-        <v>0.64</v>
+        <v>4</v>
       </c>
       <c r="K38">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="L38">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="M38">
         <v>2</v>
@@ -1682,19 +1682,19 @@
         <v>100000</v>
       </c>
       <c r="C39">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D39">
         <v>540</v>
       </c>
       <c r="E39">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F39">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G39">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H39">
         <v>10</v>
@@ -1703,13 +1703,13 @@
         <v>24</v>
       </c>
       <c r="J39">
-        <v>0.64</v>
+        <v>4</v>
       </c>
       <c r="K39">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="L39">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="M39">
         <v>2</v>
@@ -1723,19 +1723,19 @@
         <v>100000</v>
       </c>
       <c r="C40">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D40">
         <v>570</v>
       </c>
       <c r="E40">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F40">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G40">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H40">
         <v>10</v>
@@ -1744,13 +1744,13 @@
         <v>24</v>
       </c>
       <c r="J40">
-        <v>0.64</v>
+        <v>4</v>
       </c>
       <c r="K40">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="L40">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="M40">
         <v>2</v>
@@ -1764,19 +1764,19 @@
         <v>100000</v>
       </c>
       <c r="C41">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D41">
         <v>600</v>
       </c>
       <c r="E41">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F41">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G41">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H41">
         <v>10</v>
@@ -1785,13 +1785,13 @@
         <v>24</v>
       </c>
       <c r="J41">
-        <v>0.64</v>
+        <v>4</v>
       </c>
       <c r="K41">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="L41">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="M41">
         <v>2</v>
@@ -1805,19 +1805,19 @@
         <v>100000</v>
       </c>
       <c r="C43">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D43">
         <v>30</v>
       </c>
       <c r="E43">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F43">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G43">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H43">
         <v>400</v>
@@ -1829,16 +1829,16 @@
         <v>24</v>
       </c>
       <c r="K43">
-        <v>0.35</v>
+        <v>3</v>
       </c>
       <c r="L43">
-        <v>17.5</v>
+        <v>24</v>
       </c>
       <c r="M43">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="N43">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="O43">
         <v>3</v>
@@ -1852,19 +1852,19 @@
         <v>100000</v>
       </c>
       <c r="C44">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D44">
         <v>60</v>
       </c>
       <c r="E44">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F44">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G44">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H44">
         <v>400</v>
@@ -1876,16 +1876,16 @@
         <v>24</v>
       </c>
       <c r="K44">
-        <v>0.35</v>
+        <v>3</v>
       </c>
       <c r="L44">
-        <v>17.5</v>
+        <v>24</v>
       </c>
       <c r="M44">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="N44">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="O44">
         <v>3</v>
@@ -1899,19 +1899,19 @@
         <v>100000</v>
       </c>
       <c r="C45">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D45">
         <v>90</v>
       </c>
       <c r="E45">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F45">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G45">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H45">
         <v>400</v>
@@ -1923,16 +1923,16 @@
         <v>24</v>
       </c>
       <c r="K45">
-        <v>0.35</v>
+        <v>3</v>
       </c>
       <c r="L45">
-        <v>17.5</v>
+        <v>24</v>
       </c>
       <c r="M45">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="N45">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="O45">
         <v>3</v>
@@ -1946,19 +1946,19 @@
         <v>100000</v>
       </c>
       <c r="C46">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D46">
         <v>120</v>
       </c>
       <c r="E46">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F46">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G46">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H46">
         <v>400</v>
@@ -1970,16 +1970,16 @@
         <v>24</v>
       </c>
       <c r="K46">
-        <v>0.35</v>
+        <v>3</v>
       </c>
       <c r="L46">
-        <v>17.5</v>
+        <v>24</v>
       </c>
       <c r="M46">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="N46">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="O46">
         <v>3</v>
@@ -1993,19 +1993,19 @@
         <v>100000</v>
       </c>
       <c r="C47">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D47">
         <v>150</v>
       </c>
       <c r="E47">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F47">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G47">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H47">
         <v>400</v>
@@ -2017,16 +2017,16 @@
         <v>24</v>
       </c>
       <c r="K47">
-        <v>0.35</v>
+        <v>3</v>
       </c>
       <c r="L47">
-        <v>17.5</v>
+        <v>24</v>
       </c>
       <c r="M47">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="N47">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="O47">
         <v>3</v>
@@ -2040,19 +2040,19 @@
         <v>100000</v>
       </c>
       <c r="C48">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D48">
         <v>180</v>
       </c>
       <c r="E48">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F48">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G48">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H48">
         <v>400</v>
@@ -2064,16 +2064,16 @@
         <v>24</v>
       </c>
       <c r="K48">
-        <v>0.35</v>
+        <v>3</v>
       </c>
       <c r="L48">
-        <v>17.5</v>
+        <v>24</v>
       </c>
       <c r="M48">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="N48">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="O48">
         <v>3</v>
@@ -2087,19 +2087,19 @@
         <v>100000</v>
       </c>
       <c r="C49">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D49">
         <v>210</v>
       </c>
       <c r="E49">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F49">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G49">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H49">
         <v>400</v>
@@ -2111,16 +2111,16 @@
         <v>24</v>
       </c>
       <c r="K49">
-        <v>0.35</v>
+        <v>3</v>
       </c>
       <c r="L49">
-        <v>17.5</v>
+        <v>24</v>
       </c>
       <c r="M49">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="N49">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="O49">
         <v>3</v>
@@ -2134,19 +2134,19 @@
         <v>100000</v>
       </c>
       <c r="C50">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D50">
         <v>240</v>
       </c>
       <c r="E50">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F50">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G50">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H50">
         <v>400</v>
@@ -2158,16 +2158,16 @@
         <v>24</v>
       </c>
       <c r="K50">
-        <v>0.35</v>
+        <v>3</v>
       </c>
       <c r="L50">
-        <v>17.5</v>
+        <v>24</v>
       </c>
       <c r="M50">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="N50">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="O50">
         <v>3</v>
@@ -2181,19 +2181,19 @@
         <v>100000</v>
       </c>
       <c r="C51">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D51">
         <v>270</v>
       </c>
       <c r="E51">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F51">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G51">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H51">
         <v>400</v>
@@ -2205,16 +2205,16 @@
         <v>24</v>
       </c>
       <c r="K51">
-        <v>0.35</v>
+        <v>3</v>
       </c>
       <c r="L51">
-        <v>17.5</v>
+        <v>24</v>
       </c>
       <c r="M51">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="N51">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="O51">
         <v>3</v>
@@ -2228,19 +2228,19 @@
         <v>100000</v>
       </c>
       <c r="C52">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D52">
         <v>300</v>
       </c>
       <c r="E52">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F52">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G52">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H52">
         <v>400</v>
@@ -2252,16 +2252,16 @@
         <v>24</v>
       </c>
       <c r="K52">
-        <v>0.35</v>
+        <v>3</v>
       </c>
       <c r="L52">
-        <v>17.5</v>
+        <v>24</v>
       </c>
       <c r="M52">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="N52">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="O52">
         <v>3</v>
@@ -2275,19 +2275,19 @@
         <v>100000</v>
       </c>
       <c r="C53">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D53">
         <v>330</v>
       </c>
       <c r="E53">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F53">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G53">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H53">
         <v>400</v>
@@ -2299,16 +2299,16 @@
         <v>24</v>
       </c>
       <c r="K53">
-        <v>0.35</v>
+        <v>3</v>
       </c>
       <c r="L53">
-        <v>17.5</v>
+        <v>24</v>
       </c>
       <c r="M53">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="N53">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="O53">
         <v>3</v>
@@ -2322,19 +2322,19 @@
         <v>100000</v>
       </c>
       <c r="C54">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D54">
         <v>360</v>
       </c>
       <c r="E54">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F54">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G54">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H54">
         <v>400</v>
@@ -2346,16 +2346,16 @@
         <v>24</v>
       </c>
       <c r="K54">
-        <v>0.35</v>
+        <v>3</v>
       </c>
       <c r="L54">
-        <v>17.5</v>
+        <v>24</v>
       </c>
       <c r="M54">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="N54">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="O54">
         <v>3</v>
@@ -2369,19 +2369,19 @@
         <v>100000</v>
       </c>
       <c r="C55">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D55">
         <v>390</v>
       </c>
       <c r="E55">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F55">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G55">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H55">
         <v>400</v>
@@ -2393,16 +2393,16 @@
         <v>24</v>
       </c>
       <c r="K55">
-        <v>0.35</v>
+        <v>3</v>
       </c>
       <c r="L55">
-        <v>17.5</v>
+        <v>24</v>
       </c>
       <c r="M55">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="N55">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="O55">
         <v>3</v>
@@ -2416,19 +2416,19 @@
         <v>100000</v>
       </c>
       <c r="C56">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D56">
         <v>420</v>
       </c>
       <c r="E56">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F56">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G56">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H56">
         <v>400</v>
@@ -2440,16 +2440,16 @@
         <v>24</v>
       </c>
       <c r="K56">
-        <v>0.35</v>
+        <v>3</v>
       </c>
       <c r="L56">
-        <v>17.5</v>
+        <v>24</v>
       </c>
       <c r="M56">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="N56">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="O56">
         <v>3</v>
@@ -2463,19 +2463,19 @@
         <v>100000</v>
       </c>
       <c r="C57">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D57">
         <v>450</v>
       </c>
       <c r="E57">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F57">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G57">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H57">
         <v>400</v>
@@ -2487,16 +2487,16 @@
         <v>24</v>
       </c>
       <c r="K57">
-        <v>0.35</v>
+        <v>3</v>
       </c>
       <c r="L57">
-        <v>17.5</v>
+        <v>24</v>
       </c>
       <c r="M57">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="N57">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="O57">
         <v>3</v>
@@ -2510,19 +2510,19 @@
         <v>100000</v>
       </c>
       <c r="C58">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D58">
         <v>480</v>
       </c>
       <c r="E58">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F58">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G58">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H58">
         <v>400</v>
@@ -2534,16 +2534,16 @@
         <v>24</v>
       </c>
       <c r="K58">
-        <v>0.35</v>
+        <v>3</v>
       </c>
       <c r="L58">
-        <v>17.5</v>
+        <v>24</v>
       </c>
       <c r="M58">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="N58">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="O58">
         <v>3</v>
@@ -2557,19 +2557,19 @@
         <v>100000</v>
       </c>
       <c r="C59">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D59">
         <v>510</v>
       </c>
       <c r="E59">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F59">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G59">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H59">
         <v>400</v>
@@ -2581,16 +2581,16 @@
         <v>24</v>
       </c>
       <c r="K59">
-        <v>0.35</v>
+        <v>3</v>
       </c>
       <c r="L59">
-        <v>17.5</v>
+        <v>24</v>
       </c>
       <c r="M59">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="N59">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="O59">
         <v>3</v>
@@ -2604,19 +2604,19 @@
         <v>100000</v>
       </c>
       <c r="C60">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D60">
         <v>540</v>
       </c>
       <c r="E60">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F60">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G60">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H60">
         <v>400</v>
@@ -2628,16 +2628,16 @@
         <v>24</v>
       </c>
       <c r="K60">
-        <v>0.35</v>
+        <v>3</v>
       </c>
       <c r="L60">
-        <v>17.5</v>
+        <v>24</v>
       </c>
       <c r="M60">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="N60">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="O60">
         <v>3</v>
@@ -2651,19 +2651,19 @@
         <v>100000</v>
       </c>
       <c r="C61">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D61">
         <v>570</v>
       </c>
       <c r="E61">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F61">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G61">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H61">
         <v>400</v>
@@ -2675,16 +2675,16 @@
         <v>24</v>
       </c>
       <c r="K61">
-        <v>0.35</v>
+        <v>3</v>
       </c>
       <c r="L61">
-        <v>17.5</v>
+        <v>24</v>
       </c>
       <c r="M61">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="N61">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="O61">
         <v>3</v>
@@ -2698,19 +2698,19 @@
         <v>100000</v>
       </c>
       <c r="C62">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D62">
         <v>600</v>
       </c>
       <c r="E62">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F62">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="G62">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="H62">
         <v>400</v>
@@ -2722,16 +2722,16 @@
         <v>24</v>
       </c>
       <c r="K62">
-        <v>0.35</v>
+        <v>3</v>
       </c>
       <c r="L62">
-        <v>17.5</v>
+        <v>24</v>
       </c>
       <c r="M62">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="N62">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="O62">
         <v>3</v>

</xml_diff>

<commit_message>
a lot of graphes
</commit_message>
<xml_diff>
--- a/script/new_offloading.xlsx
+++ b/script/new_offloading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\BandwidthUNcertinity\script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2681CED2-EB78-4977-B4F3-63667ACDE886}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060804C3-8F49-49D8-AF9C-08CF16F17193}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="3" xr2:uid="{60046224-DB48-4D55-9DB3-CD82E3B77A28}"/>
   </bookViews>
@@ -388,8 +388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED42AF60-AB6E-40CA-87F9-E205799F0A91}">
   <dimension ref="A1:O106"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:M43"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65:H65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4509,8 +4509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{683FE496-2472-4D5D-BD1A-F7421C9B8A3B}">
   <dimension ref="A1:O106"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="O65" sqref="A65:O65"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="O68" sqref="O68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5116,10 +5116,10 @@
         <v>30</v>
       </c>
       <c r="F22">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="G22">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="H22">
         <v>10</v>
@@ -5157,10 +5157,10 @@
         <v>60</v>
       </c>
       <c r="F23">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="G23">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="H23">
         <v>10</v>
@@ -5198,10 +5198,10 @@
         <v>90</v>
       </c>
       <c r="F24">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="G24">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="H24">
         <v>10</v>
@@ -5239,10 +5239,10 @@
         <v>120</v>
       </c>
       <c r="F25">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="G25">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="H25">
         <v>10</v>
@@ -5280,10 +5280,10 @@
         <v>150</v>
       </c>
       <c r="F26">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="G26">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="H26">
         <v>10</v>
@@ -5321,10 +5321,10 @@
         <v>180</v>
       </c>
       <c r="F27">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G27">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H27">
         <v>10</v>
@@ -5362,10 +5362,10 @@
         <v>210</v>
       </c>
       <c r="F28">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="G28">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="H28">
         <v>10</v>
@@ -5403,10 +5403,10 @@
         <v>240</v>
       </c>
       <c r="F29">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G29">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="H29">
         <v>10</v>
@@ -5444,10 +5444,10 @@
         <v>270</v>
       </c>
       <c r="F30">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="G30">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H30">
         <v>10</v>
@@ -5526,10 +5526,10 @@
         <v>330</v>
       </c>
       <c r="F32">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G32">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H32">
         <v>10</v>
@@ -5567,10 +5567,10 @@
         <v>360</v>
       </c>
       <c r="F33">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G33">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="H33">
         <v>10</v>
@@ -5608,10 +5608,10 @@
         <v>390</v>
       </c>
       <c r="F34">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="G34">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="H34">
         <v>10</v>
@@ -5649,10 +5649,10 @@
         <v>420</v>
       </c>
       <c r="F35">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="G35">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="H35">
         <v>10</v>
@@ -5690,10 +5690,10 @@
         <v>450</v>
       </c>
       <c r="F36">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="G36">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="H36">
         <v>10</v>
@@ -5731,10 +5731,10 @@
         <v>480</v>
       </c>
       <c r="F37">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="G37">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="H37">
         <v>10</v>
@@ -5772,10 +5772,10 @@
         <v>510</v>
       </c>
       <c r="F38">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="G38">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="H38">
         <v>10</v>
@@ -5813,10 +5813,10 @@
         <v>540</v>
       </c>
       <c r="F39">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="G39">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="H39">
         <v>10</v>
@@ -5854,10 +5854,10 @@
         <v>570</v>
       </c>
       <c r="F40">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="G40">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="H40">
         <v>10</v>
@@ -5895,10 +5895,10 @@
         <v>600</v>
       </c>
       <c r="F41">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G41">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="H41">
         <v>10</v>
@@ -5936,10 +5936,10 @@
         <v>30</v>
       </c>
       <c r="F43">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="G43">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="H43">
         <v>10</v>
@@ -5977,10 +5977,10 @@
         <v>60</v>
       </c>
       <c r="F44">
-        <v>60</v>
+        <v>300</v>
       </c>
       <c r="G44">
-        <v>60</v>
+        <v>300</v>
       </c>
       <c r="H44">
         <v>10</v>
@@ -6018,10 +6018,10 @@
         <v>90</v>
       </c>
       <c r="F45">
-        <v>90</v>
+        <v>300</v>
       </c>
       <c r="G45">
-        <v>90</v>
+        <v>300</v>
       </c>
       <c r="H45">
         <v>10</v>
@@ -6059,10 +6059,10 @@
         <v>120</v>
       </c>
       <c r="F46">
-        <v>120</v>
+        <v>300</v>
       </c>
       <c r="G46">
-        <v>120</v>
+        <v>300</v>
       </c>
       <c r="H46">
         <v>10</v>
@@ -6100,10 +6100,10 @@
         <v>150</v>
       </c>
       <c r="F47">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="G47">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="H47">
         <v>10</v>
@@ -6141,10 +6141,10 @@
         <v>180</v>
       </c>
       <c r="F48">
-        <v>180</v>
+        <v>300</v>
       </c>
       <c r="G48">
-        <v>180</v>
+        <v>300</v>
       </c>
       <c r="H48">
         <v>10</v>
@@ -6182,10 +6182,10 @@
         <v>210</v>
       </c>
       <c r="F49">
-        <v>210</v>
+        <v>300</v>
       </c>
       <c r="G49">
-        <v>210</v>
+        <v>300</v>
       </c>
       <c r="H49">
         <v>10</v>
@@ -6223,10 +6223,10 @@
         <v>240</v>
       </c>
       <c r="F50">
-        <v>240</v>
+        <v>300</v>
       </c>
       <c r="G50">
-        <v>240</v>
+        <v>300</v>
       </c>
       <c r="H50">
         <v>10</v>
@@ -6264,10 +6264,10 @@
         <v>270</v>
       </c>
       <c r="F51">
-        <v>270</v>
+        <v>300</v>
       </c>
       <c r="G51">
-        <v>270</v>
+        <v>300</v>
       </c>
       <c r="H51">
         <v>10</v>
@@ -6346,10 +6346,10 @@
         <v>330</v>
       </c>
       <c r="F53">
-        <v>330</v>
+        <v>300</v>
       </c>
       <c r="G53">
-        <v>330</v>
+        <v>300</v>
       </c>
       <c r="H53">
         <v>10</v>
@@ -6387,10 +6387,10 @@
         <v>360</v>
       </c>
       <c r="F54">
-        <v>360</v>
+        <v>300</v>
       </c>
       <c r="G54">
-        <v>360</v>
+        <v>300</v>
       </c>
       <c r="H54">
         <v>10</v>
@@ -6428,10 +6428,10 @@
         <v>390</v>
       </c>
       <c r="F55">
-        <v>390</v>
+        <v>300</v>
       </c>
       <c r="G55">
-        <v>390</v>
+        <v>300</v>
       </c>
       <c r="H55">
         <v>10</v>
@@ -6469,10 +6469,10 @@
         <v>420</v>
       </c>
       <c r="F56">
-        <v>420</v>
+        <v>300</v>
       </c>
       <c r="G56">
-        <v>420</v>
+        <v>300</v>
       </c>
       <c r="H56">
         <v>10</v>
@@ -6510,10 +6510,10 @@
         <v>450</v>
       </c>
       <c r="F57">
-        <v>450</v>
+        <v>300</v>
       </c>
       <c r="G57">
-        <v>450</v>
+        <v>300</v>
       </c>
       <c r="H57">
         <v>10</v>
@@ -6551,10 +6551,10 @@
         <v>480</v>
       </c>
       <c r="F58">
-        <v>480</v>
+        <v>300</v>
       </c>
       <c r="G58">
-        <v>480</v>
+        <v>300</v>
       </c>
       <c r="H58">
         <v>10</v>
@@ -6592,10 +6592,10 @@
         <v>510</v>
       </c>
       <c r="F59">
-        <v>510</v>
+        <v>300</v>
       </c>
       <c r="G59">
-        <v>510</v>
+        <v>300</v>
       </c>
       <c r="H59">
         <v>10</v>
@@ -6633,10 +6633,10 @@
         <v>540</v>
       </c>
       <c r="F60">
-        <v>540</v>
+        <v>300</v>
       </c>
       <c r="G60">
-        <v>540</v>
+        <v>300</v>
       </c>
       <c r="H60">
         <v>10</v>
@@ -6674,10 +6674,10 @@
         <v>570</v>
       </c>
       <c r="F61">
-        <v>570</v>
+        <v>300</v>
       </c>
       <c r="G61">
-        <v>570</v>
+        <v>300</v>
       </c>
       <c r="H61">
         <v>10</v>
@@ -6715,10 +6715,10 @@
         <v>600</v>
       </c>
       <c r="F62">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="G62">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="H62">
         <v>10</v>
@@ -6756,13 +6756,13 @@
         <v>30</v>
       </c>
       <c r="F65">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="G65">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="H65">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="I65">
         <v>10</v>
@@ -6803,13 +6803,13 @@
         <v>60</v>
       </c>
       <c r="F66">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="G66">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="H66">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="I66">
         <v>10</v>
@@ -6850,13 +6850,13 @@
         <v>90</v>
       </c>
       <c r="F67">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="G67">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="H67">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="I67">
         <v>10</v>
@@ -6897,13 +6897,13 @@
         <v>120</v>
       </c>
       <c r="F68">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="G68">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="H68">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="I68">
         <v>10</v>
@@ -6944,13 +6944,13 @@
         <v>150</v>
       </c>
       <c r="F69">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="G69">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="H69">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="I69">
         <v>10</v>
@@ -6991,13 +6991,13 @@
         <v>180</v>
       </c>
       <c r="F70">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G70">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H70">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="I70">
         <v>10</v>
@@ -7038,13 +7038,13 @@
         <v>210</v>
       </c>
       <c r="F71">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="G71">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="H71">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="I71">
         <v>10</v>
@@ -7085,13 +7085,13 @@
         <v>240</v>
       </c>
       <c r="F72">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G72">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="H72">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="I72">
         <v>10</v>
@@ -7132,13 +7132,13 @@
         <v>270</v>
       </c>
       <c r="F73">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="G73">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H73">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="I73">
         <v>10</v>
@@ -7226,13 +7226,13 @@
         <v>330</v>
       </c>
       <c r="F75">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G75">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H75">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="I75">
         <v>10</v>
@@ -7273,13 +7273,13 @@
         <v>360</v>
       </c>
       <c r="F76">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G76">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="H76">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I76">
         <v>10</v>
@@ -7320,13 +7320,13 @@
         <v>390</v>
       </c>
       <c r="F77">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="G77">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="H77">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="I77">
         <v>10</v>
@@ -7367,13 +7367,13 @@
         <v>420</v>
       </c>
       <c r="F78">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="G78">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="H78">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="I78">
         <v>10</v>
@@ -7414,13 +7414,13 @@
         <v>450</v>
       </c>
       <c r="F79">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="G79">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="H79">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="I79">
         <v>10</v>
@@ -7461,13 +7461,13 @@
         <v>480</v>
       </c>
       <c r="F80">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="G80">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="H80">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="I80">
         <v>10</v>
@@ -7508,13 +7508,13 @@
         <v>510</v>
       </c>
       <c r="F81">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="G81">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="H81">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="I81">
         <v>10</v>
@@ -7555,13 +7555,13 @@
         <v>540</v>
       </c>
       <c r="F82">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="G82">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="H82">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="I82">
         <v>10</v>
@@ -7602,13 +7602,13 @@
         <v>570</v>
       </c>
       <c r="F83">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="G83">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="H83">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="I83">
         <v>10</v>
@@ -7649,13 +7649,13 @@
         <v>600</v>
       </c>
       <c r="F84">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G84">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="H84">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="I84">
         <v>10</v>
@@ -7696,13 +7696,13 @@
         <v>30</v>
       </c>
       <c r="F87">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="G87">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="H87">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="I87">
         <v>10</v>
@@ -7743,13 +7743,13 @@
         <v>60</v>
       </c>
       <c r="F88">
-        <v>60</v>
+        <v>300</v>
       </c>
       <c r="G88">
-        <v>60</v>
+        <v>300</v>
       </c>
       <c r="H88">
-        <v>60</v>
+        <v>300</v>
       </c>
       <c r="I88">
         <v>10</v>
@@ -7790,13 +7790,13 @@
         <v>90</v>
       </c>
       <c r="F89">
-        <v>90</v>
+        <v>300</v>
       </c>
       <c r="G89">
-        <v>90</v>
+        <v>300</v>
       </c>
       <c r="H89">
-        <v>90</v>
+        <v>300</v>
       </c>
       <c r="I89">
         <v>10</v>
@@ -7837,13 +7837,13 @@
         <v>120</v>
       </c>
       <c r="F90">
-        <v>120</v>
+        <v>300</v>
       </c>
       <c r="G90">
-        <v>120</v>
+        <v>300</v>
       </c>
       <c r="H90">
-        <v>120</v>
+        <v>300</v>
       </c>
       <c r="I90">
         <v>10</v>
@@ -7884,13 +7884,13 @@
         <v>150</v>
       </c>
       <c r="F91">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="G91">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="H91">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="I91">
         <v>10</v>
@@ -7931,13 +7931,13 @@
         <v>180</v>
       </c>
       <c r="F92">
-        <v>180</v>
+        <v>300</v>
       </c>
       <c r="G92">
-        <v>180</v>
+        <v>300</v>
       </c>
       <c r="H92">
-        <v>180</v>
+        <v>300</v>
       </c>
       <c r="I92">
         <v>10</v>
@@ -7978,13 +7978,13 @@
         <v>210</v>
       </c>
       <c r="F93">
-        <v>210</v>
+        <v>300</v>
       </c>
       <c r="G93">
-        <v>210</v>
+        <v>300</v>
       </c>
       <c r="H93">
-        <v>210</v>
+        <v>300</v>
       </c>
       <c r="I93">
         <v>10</v>
@@ -8025,13 +8025,13 @@
         <v>240</v>
       </c>
       <c r="F94">
-        <v>240</v>
+        <v>300</v>
       </c>
       <c r="G94">
-        <v>240</v>
+        <v>300</v>
       </c>
       <c r="H94">
-        <v>240</v>
+        <v>300</v>
       </c>
       <c r="I94">
         <v>10</v>
@@ -8072,13 +8072,13 @@
         <v>270</v>
       </c>
       <c r="F95">
-        <v>270</v>
+        <v>300</v>
       </c>
       <c r="G95">
-        <v>270</v>
+        <v>300</v>
       </c>
       <c r="H95">
-        <v>270</v>
+        <v>300</v>
       </c>
       <c r="I95">
         <v>10</v>
@@ -8166,13 +8166,13 @@
         <v>330</v>
       </c>
       <c r="F97">
-        <v>330</v>
+        <v>300</v>
       </c>
       <c r="G97">
-        <v>330</v>
+        <v>300</v>
       </c>
       <c r="H97">
-        <v>330</v>
+        <v>300</v>
       </c>
       <c r="I97">
         <v>10</v>
@@ -8213,13 +8213,13 @@
         <v>360</v>
       </c>
       <c r="F98">
-        <v>360</v>
+        <v>300</v>
       </c>
       <c r="G98">
-        <v>360</v>
+        <v>300</v>
       </c>
       <c r="H98">
-        <v>360</v>
+        <v>300</v>
       </c>
       <c r="I98">
         <v>10</v>
@@ -8260,13 +8260,13 @@
         <v>390</v>
       </c>
       <c r="F99">
-        <v>390</v>
+        <v>300</v>
       </c>
       <c r="G99">
-        <v>390</v>
+        <v>300</v>
       </c>
       <c r="H99">
-        <v>390</v>
+        <v>300</v>
       </c>
       <c r="I99">
         <v>10</v>
@@ -8307,13 +8307,13 @@
         <v>420</v>
       </c>
       <c r="F100">
-        <v>420</v>
+        <v>300</v>
       </c>
       <c r="G100">
-        <v>420</v>
+        <v>300</v>
       </c>
       <c r="H100">
-        <v>420</v>
+        <v>300</v>
       </c>
       <c r="I100">
         <v>10</v>
@@ -8354,13 +8354,13 @@
         <v>450</v>
       </c>
       <c r="F101">
-        <v>450</v>
+        <v>300</v>
       </c>
       <c r="G101">
-        <v>450</v>
+        <v>300</v>
       </c>
       <c r="H101">
-        <v>450</v>
+        <v>300</v>
       </c>
       <c r="I101">
         <v>10</v>
@@ -8401,13 +8401,13 @@
         <v>480</v>
       </c>
       <c r="F102">
-        <v>480</v>
+        <v>300</v>
       </c>
       <c r="G102">
-        <v>480</v>
+        <v>300</v>
       </c>
       <c r="H102">
-        <v>480</v>
+        <v>300</v>
       </c>
       <c r="I102">
         <v>10</v>
@@ -8448,13 +8448,13 @@
         <v>510</v>
       </c>
       <c r="F103">
-        <v>510</v>
+        <v>300</v>
       </c>
       <c r="G103">
-        <v>510</v>
+        <v>300</v>
       </c>
       <c r="H103">
-        <v>510</v>
+        <v>300</v>
       </c>
       <c r="I103">
         <v>10</v>
@@ -8495,13 +8495,13 @@
         <v>540</v>
       </c>
       <c r="F104">
-        <v>540</v>
+        <v>300</v>
       </c>
       <c r="G104">
-        <v>540</v>
+        <v>300</v>
       </c>
       <c r="H104">
-        <v>540</v>
+        <v>300</v>
       </c>
       <c r="I104">
         <v>10</v>
@@ -8542,13 +8542,13 @@
         <v>570</v>
       </c>
       <c r="F105">
-        <v>570</v>
+        <v>300</v>
       </c>
       <c r="G105">
-        <v>570</v>
+        <v>300</v>
       </c>
       <c r="H105">
-        <v>570</v>
+        <v>300</v>
       </c>
       <c r="I105">
         <v>10</v>
@@ -8589,13 +8589,13 @@
         <v>600</v>
       </c>
       <c r="F106">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="G106">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="H106">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="I106">
         <v>10</v>
@@ -10083,7 +10083,7 @@
   <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="F15" sqref="F15:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10282,10 +10282,10 @@
         <v>37.5</v>
       </c>
       <c r="F8">
-        <v>6.25</v>
+        <v>50</v>
       </c>
       <c r="G8">
-        <v>6.25</v>
+        <v>50</v>
       </c>
       <c r="H8">
         <v>10</v>
@@ -10323,10 +10323,10 @@
         <v>75</v>
       </c>
       <c r="F9">
-        <v>12.5</v>
+        <v>50</v>
       </c>
       <c r="G9">
-        <v>12.5</v>
+        <v>50</v>
       </c>
       <c r="H9">
         <v>10</v>
@@ -10364,10 +10364,10 @@
         <v>150</v>
       </c>
       <c r="F10">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="G10">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="H10">
         <v>10</v>
@@ -10446,10 +10446,10 @@
         <v>600</v>
       </c>
       <c r="F12">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G12">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="H12">
         <v>10</v>
@@ -10487,10 +10487,10 @@
         <v>1200</v>
       </c>
       <c r="F13">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="G13">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="H13">
         <v>10</v>
@@ -10528,10 +10528,10 @@
         <v>37.5</v>
       </c>
       <c r="F15">
-        <v>37.5</v>
+        <v>300</v>
       </c>
       <c r="G15">
-        <v>37.5</v>
+        <v>300</v>
       </c>
       <c r="H15">
         <v>10</v>
@@ -10569,10 +10569,10 @@
         <v>75</v>
       </c>
       <c r="F16">
-        <v>75</v>
+        <v>300</v>
       </c>
       <c r="G16">
-        <v>75</v>
+        <v>300</v>
       </c>
       <c r="H16">
         <v>10</v>
@@ -10610,10 +10610,10 @@
         <v>150</v>
       </c>
       <c r="F17">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="G17">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="H17">
         <v>10</v>
@@ -10692,10 +10692,10 @@
         <v>600</v>
       </c>
       <c r="F19">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="G19">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="H19">
         <v>10</v>
@@ -10733,10 +10733,10 @@
         <v>1200</v>
       </c>
       <c r="F20">
-        <v>1200</v>
+        <v>300</v>
       </c>
       <c r="G20">
-        <v>1200</v>
+        <v>300</v>
       </c>
       <c r="H20">
         <v>10</v>
@@ -10774,13 +10774,13 @@
         <v>37.5</v>
       </c>
       <c r="F22">
-        <v>6.25</v>
+        <v>50</v>
       </c>
       <c r="G22">
-        <v>6.25</v>
+        <v>50</v>
       </c>
       <c r="H22">
-        <v>6.25</v>
+        <v>50</v>
       </c>
       <c r="I22">
         <v>10</v>
@@ -10821,13 +10821,13 @@
         <v>75</v>
       </c>
       <c r="F23">
-        <v>12.5</v>
+        <v>50</v>
       </c>
       <c r="G23">
-        <v>12.5</v>
+        <v>50</v>
       </c>
       <c r="H23">
-        <v>12.5</v>
+        <v>50</v>
       </c>
       <c r="I23">
         <v>10</v>
@@ -10868,13 +10868,13 @@
         <v>150</v>
       </c>
       <c r="F24">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="G24">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="H24">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="I24">
         <v>10</v>
@@ -10962,13 +10962,13 @@
         <v>600</v>
       </c>
       <c r="F26">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G26">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="H26">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="I26">
         <v>10</v>
@@ -11009,13 +11009,13 @@
         <v>1200</v>
       </c>
       <c r="F27">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="G27">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="H27">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="I27">
         <v>10</v>
@@ -11056,13 +11056,13 @@
         <v>37.5</v>
       </c>
       <c r="F29">
-        <v>37.5</v>
+        <v>300</v>
       </c>
       <c r="G29">
-        <v>37.5</v>
+        <v>300</v>
       </c>
       <c r="H29">
-        <v>37.5</v>
+        <v>300</v>
       </c>
       <c r="I29">
         <v>10</v>
@@ -11103,13 +11103,13 @@
         <v>75</v>
       </c>
       <c r="F30">
-        <v>75</v>
+        <v>300</v>
       </c>
       <c r="G30">
-        <v>75</v>
+        <v>300</v>
       </c>
       <c r="H30">
-        <v>75</v>
+        <v>300</v>
       </c>
       <c r="I30">
         <v>10</v>
@@ -11150,13 +11150,13 @@
         <v>150</v>
       </c>
       <c r="F31">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="G31">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="H31">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="I31">
         <v>10</v>
@@ -11244,13 +11244,13 @@
         <v>600</v>
       </c>
       <c r="F33">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="G33">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="H33">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="I33">
         <v>10</v>
@@ -11291,13 +11291,13 @@
         <v>1200</v>
       </c>
       <c r="F34">
-        <v>1200</v>
+        <v>300</v>
       </c>
       <c r="G34">
-        <v>1200</v>
+        <v>300</v>
       </c>
       <c r="H34">
-        <v>1200</v>
+        <v>300</v>
       </c>
       <c r="I34">
         <v>10</v>

</xml_diff>